<commit_message>
add time stamp to excel sheet
</commit_message>
<xml_diff>
--- a/inst/app/www/Titelblatt.xlsx
+++ b/inst/app/www/Titelblatt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sszfea\GitLab\awn-tool\inst\app\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7099513F-6CEF-4E80-9E92-E73C7EEBCF8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06391ED6-3CAF-452D-8BB9-071780E4F6A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31740" yWindow="2445" windowWidth="21600" windowHeight="12735" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -42,9 +42,6 @@
     <t>T_1</t>
   </si>
   <si>
-    <t>Erstellt am</t>
-  </si>
-  <si>
     <t>Datum</t>
   </si>
   <si>
@@ -91,6 +88,9 @@
   </si>
   <si>
     <t>Eidgenössischer Gebäudeidentifikator</t>
+  </si>
+  <si>
+    <t>Datenaktualisierung:</t>
   </si>
 </sst>
 </file>
@@ -410,8 +410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -421,19 +421,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -458,10 +458,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -474,7 +474,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -488,7 +488,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -498,19 +498,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -535,10 +535,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -551,15 +551,15 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -572,7 +572,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2ECFF21-F4CD-43C7-8972-0BD700D5638B}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -583,34 +583,34 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bugfix in definitions Excel Download
</commit_message>
<xml_diff>
--- a/inst/app/www/Titelblatt.xlsx
+++ b/inst/app/www/Titelblatt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sszfea\GitLab\awn-tool\inst\app\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06391ED6-3CAF-452D-8BB9-071780E4F6A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20F736A-6EC3-4E8B-BF13-B357CFF3B77A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
   <si>
     <t>Napfgasse 6, 8022 Zürich</t>
   </si>
@@ -91,6 +91,18 @@
   </si>
   <si>
     <t>Datenaktualisierung:</t>
+  </si>
+  <si>
+    <t>Anzahl Geschosse</t>
+  </si>
+  <si>
+    <t>umfasst unter- und oberirdische Geschosse</t>
+  </si>
+  <si>
+    <t>Anzahl Zimmer</t>
+  </si>
+  <si>
+    <t>halbe Zimmer werden abgerundet</t>
   </si>
 </sst>
 </file>
@@ -410,7 +422,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -570,10 +582,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2ECFF21-F4CD-43C7-8972-0BD700D5638B}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -589,27 +601,43 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>